<commit_message>
fix: alteração e exclusão
correção de alteração e exclusão
</commit_message>
<xml_diff>
--- a/trabalho-banco/Status-funcoes.xlsx
+++ b/trabalho-banco/Status-funcoes.xlsx
@@ -1,70 +1,102 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alunos\Documents\GitHub\ILP037\trabalho-banco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F98F2B6-AAA1-46FC-AE5E-6A0092D2A125}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{05276113-DB8D-44EC-9029-C9D9BCE88173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7070" xr2:uid="{6DF090D3-2E4C-446B-817E-492BB466869E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
   <si>
     <t>Agências</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Movimentações</t>
+  </si>
+  <si>
+    <t>Incluir</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instrução insert conflitou com a restrição do foreign key "FK_MOVIMENTACAO_HIS". O conflito ocorreu na tabela "dbo.HISTORICOS", column 'ID_HIS' </t>
+  </si>
+  <si>
+    <t>Alterar</t>
+  </si>
+  <si>
+    <t>Falha ao converter data e/ou hora da cadeia de caracacteres</t>
+  </si>
+  <si>
+    <t>Excluir</t>
+  </si>
+  <si>
+    <t>não é possível deletar, tabela relacionada</t>
+  </si>
+  <si>
     <t>Clientes</t>
   </si>
   <si>
     <t>Contas Correntes</t>
   </si>
   <si>
+    <t>Conflito foreign key "fk_contacorrente_cli". O conflito ocorreu na tabela "dbo.CLIENTES", column 'ID_CLI'</t>
+  </si>
+  <si>
     <t>Históricos</t>
   </si>
   <si>
-    <t>Movimentações</t>
-  </si>
-  <si>
     <t>Usuários</t>
   </si>
   <si>
+    <t>Ler</t>
+  </si>
+  <si>
+    <t>insert conflitou com a restrição foreign key "fk_usuarios_cc". O conflito ocorreu na tabela "dbo.CONTACORRENTE"</t>
+  </si>
+  <si>
     <t>Funcionários</t>
-  </si>
-  <si>
-    <t>Incluir</t>
-  </si>
-  <si>
-    <t>Alterar</t>
-  </si>
-  <si>
-    <t>Excluir</t>
-  </si>
-  <si>
-    <t>Ler</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,7 +159,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -423,20 +455,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D642A9CA-1A59-445D-BD3B-D74457B17C5D}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="3" max="3" width="14.90625" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="129.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,79 +482,166 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>9</v>
+      <c r="B19" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>